<commit_message>
add and update workforce files
</commit_message>
<xml_diff>
--- a/Livelihoods/Employment_Figures/total labour/unemployment rate.xlsx
+++ b/Livelihoods/Employment_Figures/total labour/unemployment rate.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="11">
   <si>
     <t>Year</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Nunavut</t>
+  </si>
+  <si>
+    <t>Greenland</t>
   </si>
 </sst>
 </file>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -803,6 +806,83 @@
       </c>
       <c r="C31" s="9">
         <v>15.658333333333331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>2008</v>
+      </c>
+      <c r="C32" s="5">
+        <v>2.0410348667866014</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33">
+        <v>2009</v>
+      </c>
+      <c r="C33" s="5">
+        <v>3.640364254280859</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <v>2010</v>
+      </c>
+      <c r="C34" s="5">
+        <v>4.5763126850223701</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <v>2011</v>
+      </c>
+      <c r="C35" s="5">
+        <v>5.5478440963271414</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36">
+        <v>2012</v>
+      </c>
+      <c r="C36" s="5">
+        <v>5.9011802360472094</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>2013</v>
+      </c>
+      <c r="C37" s="5">
+        <v>6.072017469584206</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38">
+        <v>2014</v>
+      </c>
+      <c r="C38" s="5">
+        <v>6.1839003031323676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>